<commit_message>
Commit base de datos
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beecker\Pictures\Entregable\TPT.002\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beecker\Documents\UiPath\TPT.002\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8916"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -175,153 +175,6 @@
     </r>
   </si>
   <si>
-    <t>CodigoPhytonTotalBox</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Ruta PYTHON CodigoPhyton\TOTALBOX.py  No modificable Favor de agregar la misma ruta que se tiene para el campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF8EAADB"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> RutaCompartida al final de las letras rojas  despues del python</t>
-    </r>
-  </si>
-  <si>
-    <t>CodigoPhytonTpGo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Ruta PYTHON CodigoPhyton\TPGO.py  No modificable Favor de agregar la misma ruta que se tiene para el campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF8EAADB"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> RutaCompartida al final de las letras rojas  despues del python</t>
-    </r>
-  </si>
-  <si>
-    <t>CodigoPhytonHogarSeguro</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Ruta PYTHON CodigoPhyton\HOGARSEGURO.py No modificable Favor de agregar la misma ruta que se tiene para el campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF8EAADB"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> RutaCompartida al final de las letras rojas  despues del python</t>
-    </r>
-  </si>
-  <si>
-    <t>CodigoPhytonTotalPlayMX_NORTE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Ruta PYTHON CodigoPhyton\TOTALPLAYMXNORTE.py  No modificable Favor de agregar la misma ruta que se tiene para el campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF8EAADB"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> RutaCompartida al final de las letras rojas  despues del python</t>
-    </r>
-  </si>
-  <si>
-    <t>CodigoPhytonTotalBoxMX_NORTE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Ruta PYTHON CodigoPhyton\TOTALBOXMXNORTE.py  No modificable Favor de agregar la misma ruta que se tiene para el campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF8EAADB"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> RutaCompartida al final de las letras rojas  despues del python</t>
-    </r>
-  </si>
-  <si>
-    <t>CodigoPhytonTpGoMX_NORTE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Ruta PYTHON CodigoPhyton\TPGOMXNORTE.py  No modificable Favor de agregar la misma ruta que se tiene para el campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF8EAADB"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> RutaCompartida al final de las letras rojas  despues del python</t>
-    </r>
-  </si>
-  <si>
-    <t>CodigoPhytonHogarSeguroMX_NORTE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Ruta PYTHON CodigoPhyton\HOGARSEGUROMXNORTE.py  No modificable Favor de agregar la misma ruta que se tiene para el campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF8EAADB"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> RutaCompartida al final de las letras rojas  despues del python</t>
-    </r>
-  </si>
-  <si>
     <t>SalidaABC</t>
   </si>
   <si>
@@ -562,37 +415,22 @@
     <t>C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\PAGOS_PARTICION\</t>
   </si>
   <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\TOTALPLAY.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\TOTALBOX.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\TPGO.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\HOGARSEGURO.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\TOTALPLAYMXNORTE.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\TOTALBOXMXNORTE.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\TPGOMXNORTE.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\CodigoPhyton\HOGARSEGUROMXNORTE.py C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\</t>
-  </si>
-  <si>
-    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\COBRANZA\salida.abc</t>
-  </si>
-  <si>
     <t>C:\Users\Beecker\Documents\UiPath\TPT.002\Data\Output\Diferencias\DiferenciaIva.xlsx</t>
   </si>
   <si>
     <t>Hoja1</t>
+  </si>
+  <si>
+    <t>RutaCSV</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\Data\Input\CSV</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\Data\Input\CSV\salida.abc</t>
+  </si>
+  <si>
+    <t>C:\Users\Beecker\Documents\UiPath\TPT.002\Data\BD\Script_TPT_S6.py C:\Users\Beecker\Documents\UiPath\TPT.002\Data\Input\CSV\ C:\Users\Beecker\Documents\UiPath\TPT.002\Temporal\PAGOS_PARTICION\</t>
   </si>
 </sst>
 </file>
@@ -957,18 +795,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="144.6640625" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="23" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="23" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1025,7 +863,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -1036,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -1047,7 +885,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -1058,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>14</v>
@@ -1069,7 +907,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
@@ -1080,7 +918,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>17</v>
@@ -1114,7 +952,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>19</v>
@@ -1148,7 +986,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>21</v>
@@ -1159,7 +997,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>23</v>
@@ -1170,7 +1008,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>25</v>
@@ -1181,7 +1019,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>27</v>
@@ -1215,7 +1053,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>29</v>
@@ -1246,10 +1084,10 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1281,7 +1119,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>31</v>
@@ -1315,7 +1153,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>33</v>
@@ -1326,7 +1164,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>35</v>
@@ -1355,381 +1193,157 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:26" ht="15" customHeight="1">
+      <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>126</v>
+      <c r="B20" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-    </row>
-    <row r="22" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-    </row>
-    <row r="24" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="B24" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>131</v>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
+        <v>48</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" ht="15" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="3" t="s">
+    <row r="26" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
+      <c r="B26" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" ht="15" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>133</v>
+    <row r="27" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="9"/>
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:26" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A30" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
+      <c r="A30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A33" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-    </row>
-    <row r="34" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1911,13 +1525,13 @@
     <row r="227" ht="14.25" customHeight="1"/>
     <row r="228" ht="14.25" customHeight="1"/>
     <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
     <row r="237" ht="15.75" customHeight="1"/>
     <row r="238" ht="15.75" customHeight="1"/>
     <row r="239" ht="15.75" customHeight="1"/>
@@ -2676,17 +2290,10 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
     <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2699,12 +2306,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="23" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="23" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.25" customHeight="1">
@@ -2740,157 +2347,157 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="28.8">
+    <row r="3" spans="1:23" ht="30">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="43.2">
+    <row r="4" spans="1:23" ht="45">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:23" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:23" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:23" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:3" ht="28.8">
+    <row r="18" spans="1:3" ht="45">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3886,12 +3493,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="24" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="24" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" customHeight="1">
@@ -3899,13 +3506,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>

</xml_diff>